<commit_message>
user feedback import issue
</commit_message>
<xml_diff>
--- a/public/user_feedbacks_sample.xlsx
+++ b/public/user_feedbacks_sample.xlsx
@@ -5,34 +5,39 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Worksheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>answer</t>
-  </si>
-  <si>
-    <t>sandeep@ascra.com</t>
-  </si>
-  <si>
-    <t>checking percentae</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sandeep@ascra.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking percentae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
 </sst>
 </file>
@@ -40,13 +45,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+  <fonts count="7">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -69,6 +75,17 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,7 +130,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -123,6 +140,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -146,15 +171,18 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -165,24 +193,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>